<commit_message>
Se modifico el la base de datos de riesgos en el apartado de control de cambios
</commit_message>
<xml_diff>
--- a/INTyADMIN/Plaeación del proyecto/Administración de riesgos/PP_REP_v1_BD de Riesgos.xlsx
+++ b/INTyADMIN/Plaeación del proyecto/Administración de riesgos/PP_REP_v1_BD de Riesgos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\Aplicaci-n-para-control-de-cursos-de-capacitaci-n\INTyADMIN\Plaeación del proyecto\Administración de riesgos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D07D49D3-3EEA-40D8-838C-859FF2CCA1EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44075A24-1E13-4486-810A-E2678E8675D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identificación" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="548">
   <si>
     <t>Versión</t>
   </si>
@@ -1664,6 +1664,9 @@
   </si>
   <si>
     <t>0,8</t>
+  </si>
+  <si>
+    <t>Se actualizo el formato en la sección de matriz de probabilidad, ya que los datos eran erróneos, además de su operación y ubicación.</t>
   </si>
 </sst>
 </file>
@@ -2035,6 +2038,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2066,9 +2072,6 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2729,8 +2732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2818,10 +2821,10 @@
       <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="45"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="6"/>
@@ -2873,10 +2876,10 @@
       <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="45"/>
+      <c r="B22" s="46"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
     </row>
@@ -2927,12 +2930,12 @@
       <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="45"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="46"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
@@ -2976,7 +2979,20 @@
         <v>399</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:4" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="11">
+        <v>3</v>
+      </c>
+      <c r="B32" s="14">
+        <v>44056</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>547</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A16:B16"/>
@@ -5913,7 +5929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42D351A-E2DF-428B-A1AA-FF4AC66A8E66}">
   <dimension ref="A3:G208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B76" workbookViewId="0">
+    <sheetView topLeftCell="B76" workbookViewId="0">
       <selection activeCell="G100" sqref="G100"/>
     </sheetView>
   </sheetViews>
@@ -5943,40 +5959,40 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="49" t="s">
+      <c r="B11" s="55"/>
+      <c r="C11" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F11" s="49" t="s">
+      <c r="F11" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G11" s="49" t="s">
+      <c r="G11" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
     </row>
     <row r="13" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B13" s="48"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="40" t="s">
         <v>479</v>
       </c>
@@ -6030,7 +6046,7 @@
       <c r="D16" s="42"/>
       <c r="E16" s="42"/>
       <c r="F16" s="42"/>
-      <c r="G16" s="55" t="s">
+      <c r="G16" s="44" t="s">
         <v>482</v>
       </c>
     </row>
@@ -6066,40 +6082,40 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B21" s="54"/>
-      <c r="C21" s="49" t="s">
+      <c r="B21" s="55"/>
+      <c r="C21" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D21" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E21" s="49" t="s">
+      <c r="E21" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F21" s="49" t="s">
+      <c r="F21" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G21" s="49" t="s">
+      <c r="G21" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
+      <c r="A22" s="52"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B23" s="48"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="40" t="s">
         <v>479</v>
       </c>
@@ -6151,7 +6167,7 @@
       </c>
       <c r="C26" s="42"/>
       <c r="D26" s="42"/>
-      <c r="E26" s="55" t="s">
+      <c r="E26" s="44" t="s">
         <v>480</v>
       </c>
       <c r="F26" s="42"/>
@@ -6189,40 +6205,40 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="53" t="s">
+      <c r="A31" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B31" s="54"/>
-      <c r="C31" s="49" t="s">
+      <c r="B31" s="55"/>
+      <c r="C31" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D31" s="49" t="s">
+      <c r="D31" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E31" s="49" t="s">
+      <c r="E31" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F31" s="49" t="s">
+      <c r="F31" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G31" s="49" t="s">
+      <c r="G31" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="51"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
+      <c r="A32" s="52"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
     </row>
     <row r="33" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B33" s="48"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="40" t="s">
         <v>479</v>
       </c>
@@ -6312,40 +6328,40 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B41" s="54"/>
-      <c r="C41" s="49" t="s">
+      <c r="B41" s="55"/>
+      <c r="C41" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D41" s="49" t="s">
+      <c r="D41" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E41" s="49" t="s">
+      <c r="E41" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F41" s="49" t="s">
+      <c r="F41" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G41" s="49" t="s">
+      <c r="G41" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="51"/>
-      <c r="B42" s="52"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="50"/>
-      <c r="E42" s="50"/>
-      <c r="F42" s="50"/>
-      <c r="G42" s="50"/>
+      <c r="A42" s="52"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
     </row>
     <row r="43" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="47" t="s">
+      <c r="A43" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B43" s="48"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="40" t="s">
         <v>479</v>
       </c>
@@ -6435,40 +6451,40 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="53" t="s">
+      <c r="A51" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B51" s="54"/>
-      <c r="C51" s="49" t="s">
+      <c r="B51" s="55"/>
+      <c r="C51" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D51" s="49" t="s">
+      <c r="D51" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E51" s="49" t="s">
+      <c r="E51" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F51" s="49" t="s">
+      <c r="F51" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G51" s="49" t="s">
+      <c r="G51" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="51"/>
-      <c r="B52" s="52"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="50"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="50"/>
+      <c r="A52" s="52"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
     </row>
     <row r="53" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="47" t="s">
+      <c r="A53" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B53" s="48"/>
+      <c r="B53" s="49"/>
       <c r="C53" s="40" t="s">
         <v>479</v>
       </c>
@@ -6558,40 +6574,40 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="53" t="s">
+      <c r="A61" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B61" s="54"/>
-      <c r="C61" s="49" t="s">
+      <c r="B61" s="55"/>
+      <c r="C61" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D61" s="49" t="s">
+      <c r="D61" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E61" s="49" t="s">
+      <c r="E61" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F61" s="49" t="s">
+      <c r="F61" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G61" s="49" t="s">
+      <c r="G61" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="51"/>
-      <c r="B62" s="52"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="50"/>
-      <c r="E62" s="50"/>
-      <c r="F62" s="50"/>
-      <c r="G62" s="50"/>
+      <c r="A62" s="52"/>
+      <c r="B62" s="53"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="51"/>
+      <c r="E62" s="51"/>
+      <c r="F62" s="51"/>
+      <c r="G62" s="51"/>
     </row>
     <row r="63" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="47" t="s">
+      <c r="A63" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B63" s="48"/>
+      <c r="B63" s="49"/>
       <c r="C63" s="40" t="s">
         <v>479</v>
       </c>
@@ -6681,40 +6697,40 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="53" t="s">
+      <c r="A71" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B71" s="54"/>
-      <c r="C71" s="49" t="s">
+      <c r="B71" s="55"/>
+      <c r="C71" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D71" s="49" t="s">
+      <c r="D71" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E71" s="49" t="s">
+      <c r="E71" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F71" s="49" t="s">
+      <c r="F71" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G71" s="49" t="s">
+      <c r="G71" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="51"/>
-      <c r="B72" s="52"/>
-      <c r="C72" s="50"/>
-      <c r="D72" s="50"/>
-      <c r="E72" s="50"/>
-      <c r="F72" s="50"/>
-      <c r="G72" s="50"/>
+      <c r="A72" s="52"/>
+      <c r="B72" s="53"/>
+      <c r="C72" s="51"/>
+      <c r="D72" s="51"/>
+      <c r="E72" s="51"/>
+      <c r="F72" s="51"/>
+      <c r="G72" s="51"/>
     </row>
     <row r="73" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="47" t="s">
+      <c r="A73" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B73" s="48"/>
+      <c r="B73" s="49"/>
       <c r="C73" s="40" t="s">
         <v>479</v>
       </c>
@@ -6804,40 +6820,40 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="53" t="s">
+      <c r="A81" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B81" s="54"/>
-      <c r="C81" s="49" t="s">
+      <c r="B81" s="55"/>
+      <c r="C81" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D81" s="49" t="s">
+      <c r="D81" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E81" s="49" t="s">
+      <c r="E81" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F81" s="49" t="s">
+      <c r="F81" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G81" s="49" t="s">
+      <c r="G81" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="51"/>
-      <c r="B82" s="52"/>
-      <c r="C82" s="50"/>
-      <c r="D82" s="50"/>
-      <c r="E82" s="50"/>
-      <c r="F82" s="50"/>
-      <c r="G82" s="50"/>
+      <c r="A82" s="52"/>
+      <c r="B82" s="53"/>
+      <c r="C82" s="51"/>
+      <c r="D82" s="51"/>
+      <c r="E82" s="51"/>
+      <c r="F82" s="51"/>
+      <c r="G82" s="51"/>
     </row>
     <row r="83" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="47" t="s">
+      <c r="A83" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B83" s="48"/>
+      <c r="B83" s="49"/>
       <c r="C83" s="40" t="s">
         <v>479</v>
       </c>
@@ -6927,40 +6943,40 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="53" t="s">
+      <c r="A91" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B91" s="54"/>
-      <c r="C91" s="49" t="s">
+      <c r="B91" s="55"/>
+      <c r="C91" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D91" s="49" t="s">
+      <c r="D91" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E91" s="49" t="s">
+      <c r="E91" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F91" s="49" t="s">
+      <c r="F91" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G91" s="49" t="s">
+      <c r="G91" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="51"/>
-      <c r="B92" s="52"/>
-      <c r="C92" s="50"/>
-      <c r="D92" s="50"/>
-      <c r="E92" s="50"/>
-      <c r="F92" s="50"/>
-      <c r="G92" s="50"/>
+      <c r="A92" s="52"/>
+      <c r="B92" s="53"/>
+      <c r="C92" s="51"/>
+      <c r="D92" s="51"/>
+      <c r="E92" s="51"/>
+      <c r="F92" s="51"/>
+      <c r="G92" s="51"/>
     </row>
     <row r="93" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="47" t="s">
+      <c r="A93" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B93" s="48"/>
+      <c r="B93" s="49"/>
       <c r="C93" s="40" t="s">
         <v>479</v>
       </c>
@@ -7013,7 +7029,7 @@
       <c r="C96" s="42"/>
       <c r="D96" s="42"/>
       <c r="E96" s="42"/>
-      <c r="F96" s="55" t="s">
+      <c r="F96" s="44" t="s">
         <v>481</v>
       </c>
       <c r="G96" s="42"/>
@@ -7050,40 +7066,40 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="53" t="s">
+      <c r="A101" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B101" s="54"/>
-      <c r="C101" s="49" t="s">
+      <c r="B101" s="55"/>
+      <c r="C101" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D101" s="49" t="s">
+      <c r="D101" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E101" s="49" t="s">
+      <c r="E101" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F101" s="49" t="s">
+      <c r="F101" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G101" s="49" t="s">
+      <c r="G101" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="51"/>
-      <c r="B102" s="52"/>
-      <c r="C102" s="50"/>
-      <c r="D102" s="50"/>
-      <c r="E102" s="50"/>
-      <c r="F102" s="50"/>
-      <c r="G102" s="50"/>
+      <c r="A102" s="52"/>
+      <c r="B102" s="53"/>
+      <c r="C102" s="51"/>
+      <c r="D102" s="51"/>
+      <c r="E102" s="51"/>
+      <c r="F102" s="51"/>
+      <c r="G102" s="51"/>
     </row>
     <row r="103" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="47" t="s">
+      <c r="A103" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B103" s="48"/>
+      <c r="B103" s="49"/>
       <c r="C103" s="40" t="s">
         <v>479</v>
       </c>
@@ -7137,7 +7153,7 @@
       <c r="D106" s="42"/>
       <c r="E106" s="42"/>
       <c r="F106" s="42"/>
-      <c r="G106" s="55" t="s">
+      <c r="G106" s="44" t="s">
         <v>482</v>
       </c>
     </row>
@@ -7173,40 +7189,40 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" s="53" t="s">
+      <c r="A111" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B111" s="54"/>
-      <c r="C111" s="49" t="s">
+      <c r="B111" s="55"/>
+      <c r="C111" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D111" s="49" t="s">
+      <c r="D111" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E111" s="49" t="s">
+      <c r="E111" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F111" s="49" t="s">
+      <c r="F111" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G111" s="49" t="s">
+      <c r="G111" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="51"/>
-      <c r="B112" s="52"/>
-      <c r="C112" s="50"/>
-      <c r="D112" s="50"/>
-      <c r="E112" s="50"/>
-      <c r="F112" s="50"/>
-      <c r="G112" s="50"/>
+      <c r="A112" s="52"/>
+      <c r="B112" s="53"/>
+      <c r="C112" s="51"/>
+      <c r="D112" s="51"/>
+      <c r="E112" s="51"/>
+      <c r="F112" s="51"/>
+      <c r="G112" s="51"/>
     </row>
     <row r="113" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="47" t="s">
+      <c r="A113" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B113" s="48"/>
+      <c r="B113" s="49"/>
       <c r="C113" s="40" t="s">
         <v>479</v>
       </c>
@@ -7296,40 +7312,40 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A121" s="53" t="s">
+      <c r="A121" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B121" s="54"/>
-      <c r="C121" s="49" t="s">
+      <c r="B121" s="55"/>
+      <c r="C121" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D121" s="49" t="s">
+      <c r="D121" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E121" s="49" t="s">
+      <c r="E121" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F121" s="49" t="s">
+      <c r="F121" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G121" s="49" t="s">
+      <c r="G121" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="51"/>
-      <c r="B122" s="52"/>
-      <c r="C122" s="50"/>
-      <c r="D122" s="50"/>
-      <c r="E122" s="50"/>
-      <c r="F122" s="50"/>
-      <c r="G122" s="50"/>
+      <c r="A122" s="52"/>
+      <c r="B122" s="53"/>
+      <c r="C122" s="51"/>
+      <c r="D122" s="51"/>
+      <c r="E122" s="51"/>
+      <c r="F122" s="51"/>
+      <c r="G122" s="51"/>
     </row>
     <row r="123" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="47" t="s">
+      <c r="A123" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B123" s="48"/>
+      <c r="B123" s="49"/>
       <c r="C123" s="40" t="s">
         <v>479</v>
       </c>
@@ -7381,7 +7397,7 @@
       </c>
       <c r="C126" s="42"/>
       <c r="D126" s="42"/>
-      <c r="E126" s="55" t="s">
+      <c r="E126" s="44" t="s">
         <v>480</v>
       </c>
       <c r="F126" s="42"/>
@@ -7419,40 +7435,40 @@
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A131" s="53" t="s">
+      <c r="A131" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B131" s="54"/>
-      <c r="C131" s="49" t="s">
+      <c r="B131" s="55"/>
+      <c r="C131" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D131" s="49" t="s">
+      <c r="D131" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E131" s="49" t="s">
+      <c r="E131" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F131" s="49" t="s">
+      <c r="F131" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G131" s="49" t="s">
+      <c r="G131" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="51"/>
-      <c r="B132" s="52"/>
-      <c r="C132" s="50"/>
-      <c r="D132" s="50"/>
-      <c r="E132" s="50"/>
-      <c r="F132" s="50"/>
-      <c r="G132" s="50"/>
+      <c r="A132" s="52"/>
+      <c r="B132" s="53"/>
+      <c r="C132" s="51"/>
+      <c r="D132" s="51"/>
+      <c r="E132" s="51"/>
+      <c r="F132" s="51"/>
+      <c r="G132" s="51"/>
     </row>
     <row r="133" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="47" t="s">
+      <c r="A133" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B133" s="48"/>
+      <c r="B133" s="49"/>
       <c r="C133" s="40" t="s">
         <v>479</v>
       </c>
@@ -7542,40 +7558,40 @@
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A141" s="53" t="s">
+      <c r="A141" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B141" s="54"/>
-      <c r="C141" s="49" t="s">
+      <c r="B141" s="55"/>
+      <c r="C141" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D141" s="49" t="s">
+      <c r="D141" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E141" s="49" t="s">
+      <c r="E141" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F141" s="49" t="s">
+      <c r="F141" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G141" s="49" t="s">
+      <c r="G141" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="51"/>
-      <c r="B142" s="52"/>
-      <c r="C142" s="50"/>
-      <c r="D142" s="50"/>
-      <c r="E142" s="50"/>
-      <c r="F142" s="50"/>
-      <c r="G142" s="50"/>
+      <c r="A142" s="52"/>
+      <c r="B142" s="53"/>
+      <c r="C142" s="51"/>
+      <c r="D142" s="51"/>
+      <c r="E142" s="51"/>
+      <c r="F142" s="51"/>
+      <c r="G142" s="51"/>
     </row>
     <row r="143" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="47" t="s">
+      <c r="A143" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B143" s="48"/>
+      <c r="B143" s="49"/>
       <c r="C143" s="40" t="s">
         <v>479</v>
       </c>
@@ -7665,40 +7681,40 @@
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A151" s="53" t="s">
+      <c r="A151" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B151" s="54"/>
-      <c r="C151" s="49" t="s">
+      <c r="B151" s="55"/>
+      <c r="C151" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D151" s="49" t="s">
+      <c r="D151" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E151" s="49" t="s">
+      <c r="E151" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F151" s="49" t="s">
+      <c r="F151" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G151" s="49" t="s">
+      <c r="G151" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="51"/>
-      <c r="B152" s="52"/>
-      <c r="C152" s="50"/>
-      <c r="D152" s="50"/>
-      <c r="E152" s="50"/>
-      <c r="F152" s="50"/>
-      <c r="G152" s="50"/>
+      <c r="A152" s="52"/>
+      <c r="B152" s="53"/>
+      <c r="C152" s="51"/>
+      <c r="D152" s="51"/>
+      <c r="E152" s="51"/>
+      <c r="F152" s="51"/>
+      <c r="G152" s="51"/>
     </row>
     <row r="153" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="47" t="s">
+      <c r="A153" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B153" s="48"/>
+      <c r="B153" s="49"/>
       <c r="C153" s="40" t="s">
         <v>479</v>
       </c>
@@ -7788,40 +7804,40 @@
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A161" s="53" t="s">
+      <c r="A161" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B161" s="54"/>
-      <c r="C161" s="49" t="s">
+      <c r="B161" s="55"/>
+      <c r="C161" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D161" s="49" t="s">
+      <c r="D161" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E161" s="49" t="s">
+      <c r="E161" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F161" s="49" t="s">
+      <c r="F161" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G161" s="49" t="s">
+      <c r="G161" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="51"/>
-      <c r="B162" s="52"/>
-      <c r="C162" s="50"/>
-      <c r="D162" s="50"/>
-      <c r="E162" s="50"/>
-      <c r="F162" s="50"/>
-      <c r="G162" s="50"/>
+      <c r="A162" s="52"/>
+      <c r="B162" s="53"/>
+      <c r="C162" s="51"/>
+      <c r="D162" s="51"/>
+      <c r="E162" s="51"/>
+      <c r="F162" s="51"/>
+      <c r="G162" s="51"/>
     </row>
     <row r="163" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="47" t="s">
+      <c r="A163" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B163" s="48"/>
+      <c r="B163" s="49"/>
       <c r="C163" s="40" t="s">
         <v>479</v>
       </c>
@@ -7911,40 +7927,40 @@
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A171" s="53" t="s">
+      <c r="A171" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B171" s="54"/>
-      <c r="C171" s="49" t="s">
+      <c r="B171" s="55"/>
+      <c r="C171" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D171" s="49" t="s">
+      <c r="D171" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E171" s="49" t="s">
+      <c r="E171" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F171" s="49" t="s">
+      <c r="F171" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G171" s="49" t="s">
+      <c r="G171" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="51"/>
-      <c r="B172" s="52"/>
-      <c r="C172" s="50"/>
-      <c r="D172" s="50"/>
-      <c r="E172" s="50"/>
-      <c r="F172" s="50"/>
-      <c r="G172" s="50"/>
+      <c r="A172" s="52"/>
+      <c r="B172" s="53"/>
+      <c r="C172" s="51"/>
+      <c r="D172" s="51"/>
+      <c r="E172" s="51"/>
+      <c r="F172" s="51"/>
+      <c r="G172" s="51"/>
     </row>
     <row r="173" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="47" t="s">
+      <c r="A173" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B173" s="48"/>
+      <c r="B173" s="49"/>
       <c r="C173" s="40" t="s">
         <v>479</v>
       </c>
@@ -8034,40 +8050,40 @@
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A181" s="53" t="s">
+      <c r="A181" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B181" s="54"/>
-      <c r="C181" s="49" t="s">
+      <c r="B181" s="55"/>
+      <c r="C181" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D181" s="49" t="s">
+      <c r="D181" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E181" s="49" t="s">
+      <c r="E181" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F181" s="49" t="s">
+      <c r="F181" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G181" s="49" t="s">
+      <c r="G181" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="182" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="51"/>
-      <c r="B182" s="52"/>
-      <c r="C182" s="50"/>
-      <c r="D182" s="50"/>
-      <c r="E182" s="50"/>
-      <c r="F182" s="50"/>
-      <c r="G182" s="50"/>
+      <c r="A182" s="52"/>
+      <c r="B182" s="53"/>
+      <c r="C182" s="51"/>
+      <c r="D182" s="51"/>
+      <c r="E182" s="51"/>
+      <c r="F182" s="51"/>
+      <c r="G182" s="51"/>
     </row>
     <row r="183" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="47" t="s">
+      <c r="A183" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B183" s="48"/>
+      <c r="B183" s="49"/>
       <c r="C183" s="40" t="s">
         <v>479</v>
       </c>
@@ -8157,40 +8173,40 @@
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A191" s="53" t="s">
+      <c r="A191" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B191" s="54"/>
-      <c r="C191" s="49" t="s">
+      <c r="B191" s="55"/>
+      <c r="C191" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D191" s="49" t="s">
+      <c r="D191" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E191" s="49" t="s">
+      <c r="E191" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F191" s="49" t="s">
+      <c r="F191" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G191" s="49" t="s">
+      <c r="G191" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="192" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="51"/>
-      <c r="B192" s="52"/>
-      <c r="C192" s="50"/>
-      <c r="D192" s="50"/>
-      <c r="E192" s="50"/>
-      <c r="F192" s="50"/>
-      <c r="G192" s="50"/>
+      <c r="A192" s="52"/>
+      <c r="B192" s="53"/>
+      <c r="C192" s="51"/>
+      <c r="D192" s="51"/>
+      <c r="E192" s="51"/>
+      <c r="F192" s="51"/>
+      <c r="G192" s="51"/>
     </row>
     <row r="193" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="47" t="s">
+      <c r="A193" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B193" s="48"/>
+      <c r="B193" s="49"/>
       <c r="C193" s="40" t="s">
         <v>479</v>
       </c>
@@ -8280,40 +8296,40 @@
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A201" s="53" t="s">
+      <c r="A201" s="54" t="s">
         <v>472</v>
       </c>
-      <c r="B201" s="54"/>
-      <c r="C201" s="49" t="s">
+      <c r="B201" s="55"/>
+      <c r="C201" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D201" s="49" t="s">
+      <c r="D201" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E201" s="49" t="s">
+      <c r="E201" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="F201" s="49" t="s">
+      <c r="F201" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="G201" s="49" t="s">
+      <c r="G201" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="202" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="51"/>
-      <c r="B202" s="52"/>
-      <c r="C202" s="50"/>
-      <c r="D202" s="50"/>
-      <c r="E202" s="50"/>
-      <c r="F202" s="50"/>
-      <c r="G202" s="50"/>
+      <c r="A202" s="52"/>
+      <c r="B202" s="53"/>
+      <c r="C202" s="51"/>
+      <c r="D202" s="51"/>
+      <c r="E202" s="51"/>
+      <c r="F202" s="51"/>
+      <c r="G202" s="51"/>
     </row>
     <row r="203" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="47" t="s">
+      <c r="A203" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B203" s="48"/>
+      <c r="B203" s="49"/>
       <c r="C203" s="40" t="s">
         <v>479</v>
       </c>
@@ -8399,22 +8415,130 @@
     </row>
   </sheetData>
   <mergeCells count="160">
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A203:B203"/>
+    <mergeCell ref="F191:F192"/>
+    <mergeCell ref="G191:G192"/>
+    <mergeCell ref="A192:B192"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="C201:C202"/>
+    <mergeCell ref="D201:D202"/>
+    <mergeCell ref="E201:E202"/>
+    <mergeCell ref="F201:F202"/>
+    <mergeCell ref="G201:G202"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A191:B191"/>
+    <mergeCell ref="C191:C192"/>
+    <mergeCell ref="D191:D192"/>
+    <mergeCell ref="E191:E192"/>
+    <mergeCell ref="F171:F172"/>
+    <mergeCell ref="G171:G172"/>
+    <mergeCell ref="A172:B172"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A181:B181"/>
+    <mergeCell ref="C181:C182"/>
+    <mergeCell ref="D181:D182"/>
+    <mergeCell ref="E181:E182"/>
+    <mergeCell ref="F181:F182"/>
+    <mergeCell ref="G181:G182"/>
+    <mergeCell ref="A182:B182"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="A171:B171"/>
+    <mergeCell ref="C171:C172"/>
+    <mergeCell ref="D171:D172"/>
+    <mergeCell ref="E171:E172"/>
+    <mergeCell ref="F151:F152"/>
+    <mergeCell ref="G151:G152"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A161:B161"/>
+    <mergeCell ref="C161:C162"/>
+    <mergeCell ref="D161:D162"/>
+    <mergeCell ref="E161:E162"/>
+    <mergeCell ref="F161:F162"/>
+    <mergeCell ref="G161:G162"/>
+    <mergeCell ref="A162:B162"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="C151:C152"/>
+    <mergeCell ref="D151:D152"/>
+    <mergeCell ref="E151:E152"/>
+    <mergeCell ref="F131:F132"/>
+    <mergeCell ref="G131:G132"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="C141:C142"/>
+    <mergeCell ref="D141:D142"/>
+    <mergeCell ref="E141:E142"/>
+    <mergeCell ref="F141:F142"/>
+    <mergeCell ref="G141:G142"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="C131:C132"/>
+    <mergeCell ref="D131:D132"/>
+    <mergeCell ref="E131:E132"/>
+    <mergeCell ref="F111:F112"/>
+    <mergeCell ref="G111:G112"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="D121:D122"/>
+    <mergeCell ref="E121:E122"/>
+    <mergeCell ref="F121:F122"/>
+    <mergeCell ref="G121:G122"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="C111:C112"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="E111:E112"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="D101:D102"/>
+    <mergeCell ref="E101:E102"/>
+    <mergeCell ref="F101:F102"/>
+    <mergeCell ref="G101:G102"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="G81:G82"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="A62:B62"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="C51:C52"/>
@@ -8435,130 +8559,22 @@
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="E31:E32"/>
     <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="E91:E92"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="G81:G82"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="C111:C112"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="E111:E112"/>
-    <mergeCell ref="F91:F92"/>
-    <mergeCell ref="G91:G92"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="D101:D102"/>
-    <mergeCell ref="E101:E102"/>
-    <mergeCell ref="F101:F102"/>
-    <mergeCell ref="G101:G102"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="C131:C132"/>
-    <mergeCell ref="D131:D132"/>
-    <mergeCell ref="E131:E132"/>
-    <mergeCell ref="F111:F112"/>
-    <mergeCell ref="G111:G112"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="C121:C122"/>
-    <mergeCell ref="D121:D122"/>
-    <mergeCell ref="E121:E122"/>
-    <mergeCell ref="F121:F122"/>
-    <mergeCell ref="G121:G122"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="C151:C152"/>
-    <mergeCell ref="D151:D152"/>
-    <mergeCell ref="E151:E152"/>
-    <mergeCell ref="F131:F132"/>
-    <mergeCell ref="G131:G132"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="C141:C142"/>
-    <mergeCell ref="D141:D142"/>
-    <mergeCell ref="E141:E142"/>
-    <mergeCell ref="F141:F142"/>
-    <mergeCell ref="G141:G142"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="A171:B171"/>
-    <mergeCell ref="C171:C172"/>
-    <mergeCell ref="D171:D172"/>
-    <mergeCell ref="E171:E172"/>
-    <mergeCell ref="F151:F152"/>
-    <mergeCell ref="G151:G152"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A161:B161"/>
-    <mergeCell ref="C161:C162"/>
-    <mergeCell ref="D161:D162"/>
-    <mergeCell ref="E161:E162"/>
-    <mergeCell ref="F161:F162"/>
-    <mergeCell ref="G161:G162"/>
-    <mergeCell ref="A162:B162"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A191:B191"/>
-    <mergeCell ref="C191:C192"/>
-    <mergeCell ref="D191:D192"/>
-    <mergeCell ref="E191:E192"/>
-    <mergeCell ref="F171:F172"/>
-    <mergeCell ref="G171:G172"/>
-    <mergeCell ref="A172:B172"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A181:B181"/>
-    <mergeCell ref="C181:C182"/>
-    <mergeCell ref="D181:D182"/>
-    <mergeCell ref="E181:E182"/>
-    <mergeCell ref="F181:F182"/>
-    <mergeCell ref="G181:G182"/>
-    <mergeCell ref="A182:B182"/>
-    <mergeCell ref="A203:B203"/>
-    <mergeCell ref="F191:F192"/>
-    <mergeCell ref="G191:G192"/>
-    <mergeCell ref="A192:B192"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="C201:C202"/>
-    <mergeCell ref="D201:D202"/>
-    <mergeCell ref="E201:E202"/>
-    <mergeCell ref="F201:F202"/>
-    <mergeCell ref="G201:G202"/>
-    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>